<commit_message>
built volun filter, need modify
</commit_message>
<xml_diff>
--- a/uploads/2021_Learning_Destination_2.xlsx
+++ b/uploads/2021_Learning_Destination_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lincoln Uni\Computing\639\pj2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C4D57A-A01A-45C6-AFBC-81CCED6B0BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C2594F-FD34-4595-9494-28E9CD2E00A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="56">
   <si>
     <t>Paperwork</t>
   </si>
@@ -118,6 +118,9 @@
     <t>$46.00</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>Received</t>
   </si>
   <si>
@@ -158,15 +161,43 @@
   </si>
   <si>
     <t>$15.00</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>lll</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>ddddd</t>
+  </si>
+  <si>
+    <t>sssss</t>
+  </si>
+  <si>
+    <t>ccccc</t>
+  </si>
+  <si>
+    <t>eee</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -246,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -270,20 +301,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -602,10 +630,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AI12"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,15 +651,14 @@
     <col min="18" max="18" width="10.5546875" customWidth="1"/>
     <col min="19" max="20" width="12.109375" customWidth="1"/>
     <col min="21" max="21" width="13.44140625" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="U1" s="12" t="s">
+    <row r="1" spans="1:24" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="U1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -695,32 +722,21 @@
       <c r="U2" s="2">
         <v>2020</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2">
         <v>2021</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2">
         <v>2022</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2">
         <v>2023</v>
       </c>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
-      <c r="AG2" s="2"/>
-      <c r="AH2" s="2"/>
-      <c r="AI2" s="2"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
-        <v>10041</v>
-      </c>
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>10049</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -762,63 +778,69 @@
       <c r="O3" s="4">
         <v>43501</v>
       </c>
-      <c r="P3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R3" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S3" s="2" t="b">
-        <v>1</v>
+      <c r="P3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="V3" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="V3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X3" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
-        <v>10042</v>
-      </c>
-      <c r="B4" s="11" t="s">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>10050</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N4" s="4">
         <v>43503</v>
@@ -826,42 +848,48 @@
       <c r="O4" s="4">
         <v>43503</v>
       </c>
-      <c r="P4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4" s="2" t="b">
-        <v>1</v>
+      <c r="P4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V4" t="s">
         <v>33</v>
       </c>
-      <c r="V4" s="2" t="s">
-        <v>32</v>
+      <c r="W4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:35" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
-        <v>10043</v>
+    <row r="5" spans="1:24" s="8" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>10051</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5"/>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
         <v>26</v>
@@ -870,13 +898,13 @@
       <c r="I5"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N5" s="4">
         <v>43546</v>
@@ -884,35 +912,407 @@
       <c r="O5" s="4">
         <v>43181</v>
       </c>
-      <c r="P5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="R5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="S5" s="10" t="b">
-        <v>1</v>
+      <c r="P5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="T5" s="10"/>
       <c r="U5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W5" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>10052</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V6" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" t="s">
+        <v>34</v>
+      </c>
+      <c r="X6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>10053</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N7" s="15">
+        <v>43501</v>
+      </c>
+      <c r="O7" s="15">
+        <v>43501</v>
+      </c>
+      <c r="P7" t="s">
         <v>32</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="Q7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R7" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U7" t="s">
         <v>33</v>
       </c>
+      <c r="V7" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" t="s">
+        <v>34</v>
+      </c>
+      <c r="X7" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>10054</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="15">
+        <v>43503</v>
+      </c>
+      <c r="O8" s="15">
+        <v>43503</v>
+      </c>
+      <c r="P8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" t="s">
+        <v>34</v>
+      </c>
+      <c r="S8" t="s">
+        <v>34</v>
+      </c>
+      <c r="U8" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" t="s">
+        <v>33</v>
+      </c>
+      <c r="W8" t="s">
+        <v>34</v>
+      </c>
+      <c r="X8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>10055</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" s="15">
+        <v>43546</v>
+      </c>
+      <c r="O9" s="15">
+        <v>43181</v>
+      </c>
+      <c r="P9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" t="s">
+        <v>32</v>
+      </c>
+      <c r="S9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" t="s">
+        <v>33</v>
+      </c>
+      <c r="V9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W9" t="s">
+        <v>34</v>
+      </c>
+      <c r="X9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10056</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" t="s">
+        <v>34</v>
+      </c>
+      <c r="S10" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" t="s">
+        <v>34</v>
+      </c>
+      <c r="V10" t="s">
+        <v>34</v>
+      </c>
+      <c r="W10" t="s">
+        <v>34</v>
+      </c>
+      <c r="X10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10057</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="L11" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" t="s">
+        <v>40</v>
+      </c>
+      <c r="P11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" t="s">
+        <v>34</v>
+      </c>
+      <c r="V11" t="s">
+        <v>34</v>
+      </c>
+      <c r="W11" t="s">
+        <v>34</v>
+      </c>
+      <c r="X11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B12:D12"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape"/>
 </worksheet>

</xml_diff>